<commit_message>
Add lab 2.5.1 report
</commit_message>
<xml_diff>
--- a/2sem/labs/2.5.1/process/data_normal.xlsx
+++ b/2sem/labs/2.5.1/process/data_normal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mipt_edu\2sem\labs\2.5.1\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D6F368-E502-4CE5-BE6E-E011C23A37CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5590CA2-A704-42AA-B741-28A9A98ABCC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -397,7 +397,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="42" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,10 +482,10 @@
         <v>0.01</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3" t="s">
         <v>2</v>
@@ -680,6 +680,50 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{43974476-1B6E-4F7D-8FD1-3F387B7B97D3}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'L1'!L16:L16</xm:f>
+              <xm:sqref>K16</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'L1'!L17:L17</xm:f>
+              <xm:sqref>K17</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'L1'!L18:L18</xm:f>
+              <xm:sqref>K18</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'L1'!L19:L19</xm:f>
+              <xm:sqref>K19</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'L1'!L20:L20</xm:f>
+              <xm:sqref>K20</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'L1'!L21:L21</xm:f>
+              <xm:sqref>K21</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'L1'!L22:L22</xm:f>
+              <xm:sqref>K22</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'L1'!L23:L23</xm:f>
+              <xm:sqref>K23</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{0917E53A-92EC-4790-B41B-904D7A2926F8}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
@@ -724,50 +768,6 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{43974476-1B6E-4F7D-8FD1-3F387B7B97D3}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'L1'!L16:L16</xm:f>
-              <xm:sqref>K16</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'L1'!L17:L17</xm:f>
-              <xm:sqref>K17</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'L1'!L18:L18</xm:f>
-              <xm:sqref>K18</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'L1'!L19:L19</xm:f>
-              <xm:sqref>K19</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'L1'!L20:L20</xm:f>
-              <xm:sqref>K20</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'L1'!L21:L21</xm:f>
-              <xm:sqref>K21</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'L1'!L22:L22</xm:f>
-              <xm:sqref>K22</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'L1'!L23:L23</xm:f>
-              <xm:sqref>K23</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>

</xml_diff>